<commit_message>
feat: subject view updated.
</commit_message>
<xml_diff>
--- a/src/Web/SchoolAttendance.WebAPI/ExcelTemplates/Upload/1. Subjects.xlsx
+++ b/src/Web/SchoolAttendance.WebAPI/ExcelTemplates/Upload/1. Subjects.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e7e5cc81f06df1e3/Desktop/Excel Templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Dynami-Projects\School-Mangements\SchoolAttendance\src\Web\SchoolAttendance.WebAPI\ExcelTemplates\Upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{3AD4C3FF-5097-408B-A62C-FFF8173D5DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EAB870A6-06F3-4E61-95A3-C814934C3FED}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3644CEC6-0529-48E6-A63C-462A98FADACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{951120F8-1995-4E72-9D91-7230F985DAEA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{951120F8-1995-4E72-9D91-7230F985DAEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Subjects" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,6 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="22">
   <si>
     <t>SubjectName</t>
   </si>
@@ -51,6 +50,54 @@
   </si>
   <si>
     <t>DepartmentHead</t>
+  </si>
+  <si>
+    <t>ParentSubjectName</t>
+  </si>
+  <si>
+    <t>Sinhala</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Science</t>
+  </si>
+  <si>
+    <t>Mathematics</t>
+  </si>
+  <si>
+    <t>Geography</t>
+  </si>
+  <si>
+    <t>History</t>
+  </si>
+  <si>
+    <t>Tamil</t>
+  </si>
+  <si>
+    <t>Civics</t>
+  </si>
+  <si>
+    <t>English Lit.</t>
+  </si>
+  <si>
+    <t>Health &amp; Phy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PTS </t>
+  </si>
+  <si>
+    <t>Art Subject</t>
+  </si>
+  <si>
+    <t>Music</t>
+  </si>
+  <si>
+    <t>Dancing</t>
+  </si>
+  <si>
+    <t>Art</t>
   </si>
 </sst>
 </file>
@@ -82,7 +129,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -152,6 +199,43 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -167,13 +251,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,22 +575,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{560EC16E-FF73-4B15-B358-5144F7DEA6B5}">
-  <dimension ref="A1:F166"/>
+  <dimension ref="A1:G166"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
-    <col min="4" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="4" max="5" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" customWidth="1"/>
+    <col min="7" max="7" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -522,1326 +610,1650 @@
       <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
+      <c r="G1" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="6">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="7">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="7">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="7">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="7">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="7">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="7">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="7">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="7">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="7">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="7">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="7">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="7">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+      <c r="F15" s="7">
+        <v>1</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E16" s="1">
+        <v>0</v>
+      </c>
+      <c r="F16" s="7">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="7"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F18" s="7"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F19" s="7"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F20" s="7"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F21" s="7"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F22" s="7"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F23" s="7"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F24" s="7"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F25" s="7"/>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F26" s="7"/>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F27" s="7"/>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F28" s="7"/>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F29" s="7"/>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F30" s="7"/>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F31" s="7"/>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F32" s="7"/>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F33" s="7"/>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F34" s="7"/>
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F35" s="7"/>
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F36" s="7"/>
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F37" s="7"/>
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F38" s="7"/>
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F39" s="7"/>
+      <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F40" s="7"/>
+      <c r="G40" s="1"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F41" s="7"/>
+      <c r="G41" s="1"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F42" s="7"/>
+      <c r="G42" s="1"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F43" s="7"/>
+      <c r="G43" s="1"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F44" s="7"/>
+      <c r="G44" s="1"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F45" s="7"/>
+      <c r="G45" s="1"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F46" s="7"/>
+      <c r="G46" s="1"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F47" s="7"/>
+      <c r="G47" s="1"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F48" s="7"/>
+      <c r="G48" s="1"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F49" s="7"/>
+      <c r="G49" s="1"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F50" s="7"/>
+      <c r="G50" s="1"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F51" s="7"/>
+      <c r="G51" s="1"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F52" s="7"/>
+      <c r="G52" s="1"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F53" s="7"/>
+      <c r="G53" s="1"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F54" s="7"/>
+      <c r="G54" s="1"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F55" s="7"/>
+      <c r="G55" s="1"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F56" s="7"/>
+      <c r="G56" s="1"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
-      <c r="F57" s="1"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F57" s="7"/>
+      <c r="G57" s="1"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F58" s="7"/>
+      <c r="G58" s="1"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
-      <c r="F59" s="1"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F59" s="7"/>
+      <c r="G59" s="1"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
-      <c r="F60" s="1"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F60" s="7"/>
+      <c r="G60" s="1"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
-      <c r="F61" s="1"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F61" s="7"/>
+      <c r="G61" s="1"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
-      <c r="F62" s="1"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F62" s="7"/>
+      <c r="G62" s="1"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
-      <c r="F63" s="1"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F63" s="7"/>
+      <c r="G63" s="1"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
-      <c r="F64" s="1"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F64" s="7"/>
+      <c r="G64" s="1"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
-      <c r="F65" s="1"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F65" s="7"/>
+      <c r="G65" s="1"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
-      <c r="F66" s="1"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F66" s="7"/>
+      <c r="G66" s="1"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
-      <c r="F67" s="1"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F67" s="7"/>
+      <c r="G67" s="1"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
-      <c r="F68" s="1"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F68" s="7"/>
+      <c r="G68" s="1"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F69" s="7"/>
+      <c r="G69" s="1"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F70" s="7"/>
+      <c r="G70" s="1"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
-      <c r="F71" s="1"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F71" s="7"/>
+      <c r="G71" s="1"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
-      <c r="F72" s="1"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F72" s="7"/>
+      <c r="G72" s="1"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
-      <c r="F73" s="1"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F73" s="7"/>
+      <c r="G73" s="1"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
-      <c r="F74" s="1"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F74" s="7"/>
+      <c r="G74" s="1"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
-      <c r="F75" s="1"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F75" s="7"/>
+      <c r="G75" s="1"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
-      <c r="F76" s="1"/>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F76" s="7"/>
+      <c r="G76" s="1"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
-      <c r="F77" s="1"/>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F77" s="7"/>
+      <c r="G77" s="1"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
-      <c r="F78" s="1"/>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F78" s="7"/>
+      <c r="G78" s="1"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
-      <c r="F79" s="1"/>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F79" s="7"/>
+      <c r="G79" s="1"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
-      <c r="F80" s="1"/>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F80" s="7"/>
+      <c r="G80" s="1"/>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
-      <c r="F81" s="1"/>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F81" s="7"/>
+      <c r="G81" s="1"/>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
-      <c r="F82" s="1"/>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F82" s="7"/>
+      <c r="G82" s="1"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
-      <c r="F83" s="1"/>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F83" s="7"/>
+      <c r="G83" s="1"/>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
-      <c r="F84" s="1"/>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F84" s="7"/>
+      <c r="G84" s="1"/>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
-      <c r="F85" s="1"/>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F85" s="7"/>
+      <c r="G85" s="1"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
-      <c r="F86" s="1"/>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F86" s="7"/>
+      <c r="G86" s="1"/>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
-      <c r="F87" s="1"/>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F87" s="7"/>
+      <c r="G87" s="1"/>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
-      <c r="F88" s="1"/>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F88" s="7"/>
+      <c r="G88" s="1"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
-      <c r="F89" s="1"/>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F89" s="7"/>
+      <c r="G89" s="1"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
-      <c r="F90" s="1"/>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F90" s="7"/>
+      <c r="G90" s="1"/>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
-      <c r="F91" s="1"/>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F91" s="7"/>
+      <c r="G91" s="1"/>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
-      <c r="F92" s="1"/>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F92" s="7"/>
+      <c r="G92" s="1"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
-      <c r="F93" s="1"/>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F93" s="7"/>
+      <c r="G93" s="1"/>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
-      <c r="F94" s="1"/>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F94" s="7"/>
+      <c r="G94" s="1"/>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
       <c r="E95" s="1"/>
-      <c r="F95" s="1"/>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F95" s="7"/>
+      <c r="G95" s="1"/>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
       <c r="E96" s="1"/>
-      <c r="F96" s="1"/>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F96" s="7"/>
+      <c r="G96" s="1"/>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
-      <c r="F97" s="1"/>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F97" s="7"/>
+      <c r="G97" s="1"/>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
-      <c r="F98" s="1"/>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F98" s="7"/>
+      <c r="G98" s="1"/>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
-      <c r="F99" s="1"/>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F99" s="7"/>
+      <c r="G99" s="1"/>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
       <c r="E100" s="1"/>
-      <c r="F100" s="1"/>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F100" s="7"/>
+      <c r="G100" s="1"/>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
       <c r="E101" s="1"/>
-      <c r="F101" s="1"/>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F101" s="7"/>
+      <c r="G101" s="1"/>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
-      <c r="F102" s="1"/>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F102" s="7"/>
+      <c r="G102" s="1"/>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
       <c r="E103" s="1"/>
-      <c r="F103" s="1"/>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F103" s="7"/>
+      <c r="G103" s="1"/>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
       <c r="E104" s="1"/>
-      <c r="F104" s="1"/>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F104" s="7"/>
+      <c r="G104" s="1"/>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
       <c r="D105" s="1"/>
       <c r="E105" s="1"/>
-      <c r="F105" s="1"/>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F105" s="7"/>
+      <c r="G105" s="1"/>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
       <c r="E106" s="1"/>
-      <c r="F106" s="1"/>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F106" s="7"/>
+      <c r="G106" s="1"/>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
       <c r="E107" s="1"/>
-      <c r="F107" s="1"/>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F107" s="7"/>
+      <c r="G107" s="1"/>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
       <c r="D108" s="1"/>
       <c r="E108" s="1"/>
-      <c r="F108" s="1"/>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F108" s="7"/>
+      <c r="G108" s="1"/>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
       <c r="E109" s="1"/>
-      <c r="F109" s="1"/>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F109" s="7"/>
+      <c r="G109" s="1"/>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
       <c r="E110" s="1"/>
-      <c r="F110" s="1"/>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F110" s="7"/>
+      <c r="G110" s="1"/>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
       <c r="D111" s="1"/>
       <c r="E111" s="1"/>
-      <c r="F111" s="1"/>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F111" s="7"/>
+      <c r="G111" s="1"/>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
       <c r="D112" s="1"/>
       <c r="E112" s="1"/>
-      <c r="F112" s="1"/>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F112" s="7"/>
+      <c r="G112" s="1"/>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
       <c r="D113" s="1"/>
       <c r="E113" s="1"/>
-      <c r="F113" s="1"/>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F113" s="7"/>
+      <c r="G113" s="1"/>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
       <c r="D114" s="1"/>
       <c r="E114" s="1"/>
-      <c r="F114" s="1"/>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F114" s="7"/>
+      <c r="G114" s="1"/>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
       <c r="D115" s="1"/>
       <c r="E115" s="1"/>
-      <c r="F115" s="1"/>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F115" s="7"/>
+      <c r="G115" s="1"/>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
       <c r="D116" s="1"/>
       <c r="E116" s="1"/>
-      <c r="F116" s="1"/>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F116" s="7"/>
+      <c r="G116" s="1"/>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
       <c r="E117" s="1"/>
-      <c r="F117" s="1"/>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F117" s="7"/>
+      <c r="G117" s="1"/>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
       <c r="D118" s="1"/>
       <c r="E118" s="1"/>
-      <c r="F118" s="1"/>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F118" s="7"/>
+      <c r="G118" s="1"/>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
       <c r="D119" s="1"/>
       <c r="E119" s="1"/>
-      <c r="F119" s="1"/>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F119" s="7"/>
+      <c r="G119" s="1"/>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
       <c r="D120" s="1"/>
       <c r="E120" s="1"/>
-      <c r="F120" s="1"/>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F120" s="7"/>
+      <c r="G120" s="1"/>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
       <c r="D121" s="1"/>
       <c r="E121" s="1"/>
-      <c r="F121" s="1"/>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F121" s="7"/>
+      <c r="G121" s="1"/>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
       <c r="D122" s="1"/>
       <c r="E122" s="1"/>
-      <c r="F122" s="1"/>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F122" s="7"/>
+      <c r="G122" s="1"/>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
       <c r="D123" s="1"/>
       <c r="E123" s="1"/>
-      <c r="F123" s="1"/>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F123" s="7"/>
+      <c r="G123" s="1"/>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
       <c r="D124" s="1"/>
       <c r="E124" s="1"/>
-      <c r="F124" s="1"/>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F124" s="7"/>
+      <c r="G124" s="1"/>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
       <c r="D125" s="1"/>
       <c r="E125" s="1"/>
-      <c r="F125" s="1"/>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F125" s="7"/>
+      <c r="G125" s="1"/>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
       <c r="D126" s="1"/>
       <c r="E126" s="1"/>
-      <c r="F126" s="1"/>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F126" s="7"/>
+      <c r="G126" s="1"/>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
       <c r="D127" s="1"/>
       <c r="E127" s="1"/>
-      <c r="F127" s="1"/>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F127" s="7"/>
+      <c r="G127" s="1"/>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
       <c r="D128" s="1"/>
       <c r="E128" s="1"/>
-      <c r="F128" s="1"/>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F128" s="7"/>
+      <c r="G128" s="1"/>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
       <c r="D129" s="1"/>
       <c r="E129" s="1"/>
-      <c r="F129" s="1"/>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F129" s="7"/>
+      <c r="G129" s="1"/>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
       <c r="D130" s="1"/>
       <c r="E130" s="1"/>
-      <c r="F130" s="1"/>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F130" s="7"/>
+      <c r="G130" s="1"/>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
       <c r="D131" s="1"/>
       <c r="E131" s="1"/>
-      <c r="F131" s="1"/>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F131" s="7"/>
+      <c r="G131" s="1"/>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
       <c r="D132" s="1"/>
       <c r="E132" s="1"/>
-      <c r="F132" s="1"/>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F132" s="7"/>
+      <c r="G132" s="1"/>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
       <c r="D133" s="1"/>
       <c r="E133" s="1"/>
-      <c r="F133" s="1"/>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F133" s="7"/>
+      <c r="G133" s="1"/>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
       <c r="D134" s="1"/>
       <c r="E134" s="1"/>
-      <c r="F134" s="1"/>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F134" s="7"/>
+      <c r="G134" s="1"/>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
       <c r="D135" s="1"/>
       <c r="E135" s="1"/>
-      <c r="F135" s="1"/>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F135" s="7"/>
+      <c r="G135" s="1"/>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
       <c r="D136" s="1"/>
       <c r="E136" s="1"/>
-      <c r="F136" s="1"/>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F136" s="7"/>
+      <c r="G136" s="1"/>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
       <c r="D137" s="1"/>
       <c r="E137" s="1"/>
-      <c r="F137" s="1"/>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F137" s="7"/>
+      <c r="G137" s="1"/>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
       <c r="D138" s="1"/>
       <c r="E138" s="1"/>
-      <c r="F138" s="1"/>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F138" s="7"/>
+      <c r="G138" s="1"/>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
       <c r="D139" s="1"/>
       <c r="E139" s="1"/>
-      <c r="F139" s="1"/>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F139" s="7"/>
+      <c r="G139" s="1"/>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
       <c r="D140" s="1"/>
       <c r="E140" s="1"/>
-      <c r="F140" s="1"/>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F140" s="7"/>
+      <c r="G140" s="1"/>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
       <c r="D141" s="1"/>
       <c r="E141" s="1"/>
-      <c r="F141" s="1"/>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F141" s="7"/>
+      <c r="G141" s="1"/>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
       <c r="D142" s="1"/>
       <c r="E142" s="1"/>
-      <c r="F142" s="1"/>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F142" s="7"/>
+      <c r="G142" s="1"/>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
       <c r="D143" s="1"/>
       <c r="E143" s="1"/>
-      <c r="F143" s="1"/>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F143" s="7"/>
+      <c r="G143" s="1"/>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
       <c r="D144" s="1"/>
       <c r="E144" s="1"/>
-      <c r="F144" s="1"/>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F144" s="7"/>
+      <c r="G144" s="1"/>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
       <c r="D145" s="1"/>
       <c r="E145" s="1"/>
-      <c r="F145" s="1"/>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F145" s="7"/>
+      <c r="G145" s="1"/>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
       <c r="D146" s="1"/>
       <c r="E146" s="1"/>
-      <c r="F146" s="1"/>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F146" s="7"/>
+      <c r="G146" s="1"/>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
       <c r="D147" s="1"/>
       <c r="E147" s="1"/>
-      <c r="F147" s="1"/>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F147" s="7"/>
+      <c r="G147" s="1"/>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
       <c r="D148" s="1"/>
       <c r="E148" s="1"/>
-      <c r="F148" s="1"/>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F148" s="7"/>
+      <c r="G148" s="1"/>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
       <c r="D149" s="1"/>
       <c r="E149" s="1"/>
-      <c r="F149" s="1"/>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F149" s="7"/>
+      <c r="G149" s="1"/>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
       <c r="D150" s="1"/>
       <c r="E150" s="1"/>
-      <c r="F150" s="1"/>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F150" s="7"/>
+      <c r="G150" s="1"/>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
       <c r="D151" s="1"/>
       <c r="E151" s="1"/>
-      <c r="F151" s="1"/>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F151" s="7"/>
+      <c r="G151" s="1"/>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
       <c r="D152" s="1"/>
       <c r="E152" s="1"/>
-      <c r="F152" s="1"/>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F152" s="7"/>
+      <c r="G152" s="1"/>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
       <c r="D153" s="1"/>
       <c r="E153" s="1"/>
-      <c r="F153" s="1"/>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F153" s="7"/>
+      <c r="G153" s="1"/>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
       <c r="D154" s="1"/>
       <c r="E154" s="1"/>
-      <c r="F154" s="1"/>
-    </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F154" s="7"/>
+      <c r="G154" s="1"/>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
       <c r="D155" s="1"/>
       <c r="E155" s="1"/>
-      <c r="F155" s="1"/>
-    </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F155" s="7"/>
+      <c r="G155" s="1"/>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
       <c r="D156" s="1"/>
       <c r="E156" s="1"/>
-      <c r="F156" s="1"/>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F156" s="7"/>
+      <c r="G156" s="1"/>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
       <c r="D157" s="1"/>
       <c r="E157" s="1"/>
-      <c r="F157" s="1"/>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F157" s="7"/>
+      <c r="G157" s="1"/>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
       <c r="D158" s="1"/>
       <c r="E158" s="1"/>
-      <c r="F158" s="1"/>
-    </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F158" s="7"/>
+      <c r="G158" s="1"/>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
       <c r="D159" s="1"/>
       <c r="E159" s="1"/>
-      <c r="F159" s="1"/>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F159" s="7"/>
+      <c r="G159" s="1"/>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
       <c r="D160" s="1"/>
       <c r="E160" s="1"/>
-      <c r="F160" s="1"/>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F160" s="7"/>
+      <c r="G160" s="1"/>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
       <c r="D161" s="1"/>
       <c r="E161" s="1"/>
-      <c r="F161" s="1"/>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F161" s="7"/>
+      <c r="G161" s="1"/>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
       <c r="D162" s="1"/>
       <c r="E162" s="1"/>
-      <c r="F162" s="1"/>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F162" s="7"/>
+      <c r="G162" s="1"/>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
       <c r="D163" s="1"/>
       <c r="E163" s="1"/>
-      <c r="F163" s="1"/>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F163" s="7"/>
+      <c r="G163" s="1"/>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
       <c r="D164" s="1"/>
       <c r="E164" s="1"/>
-      <c r="F164" s="1"/>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F164" s="7"/>
+      <c r="G164" s="1"/>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
       <c r="D165" s="1"/>
       <c r="E165" s="1"/>
-      <c r="F165" s="1"/>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F165" s="7"/>
+      <c r="G165" s="1"/>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
       <c r="D166" s="1"/>
       <c r="E166" s="1"/>
-      <c r="F166" s="1"/>
+      <c r="F166" s="7"/>
+      <c r="G166" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>